<commit_message>
Updated to include more events and a few races that were missed
</commit_message>
<xml_diff>
--- a/GTA_EVENTS_TABLE.xlsx
+++ b/GTA_EVENTS_TABLE.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Curtis\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Curtis\Desktop\GTA_Playlist_Builder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65E09AA8-282E-4225-8704-7D407854C679}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{210F55A8-91DA-4584-9467-A229C7ECE6CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EAFCA132-E104-414E-9878-84222FD960B1}"/>
+    <workbookView xWindow="1140" yWindow="1605" windowWidth="27660" windowHeight="13995" xr2:uid="{EAFCA132-E104-414E-9878-84222FD960B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,20 +33,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
-  <si>
-    <t>Hunting Pack</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="40">
   <si>
     <t>event_name</t>
   </si>
   <si>
-    <t>Stunters Vs Snipers</t>
-  </si>
-  <si>
-    <t>Runners Vs Zentornos</t>
-  </si>
-  <si>
     <t>LTS</t>
   </si>
   <si>
@@ -99,6 +90,69 @@
   </si>
   <si>
     <t>Bikes vs RPG</t>
+  </si>
+  <si>
+    <t>Sumo I</t>
+  </si>
+  <si>
+    <t>Sumo II</t>
+  </si>
+  <si>
+    <t>Sumo III</t>
+  </si>
+  <si>
+    <t>Adversary</t>
+  </si>
+  <si>
+    <t>Sumo (Remix) I</t>
+  </si>
+  <si>
+    <t>Sumo (Remix) II</t>
+  </si>
+  <si>
+    <t>Sumo (Remix) III</t>
+  </si>
+  <si>
+    <t>Sumo (Remix) IV</t>
+  </si>
+  <si>
+    <t>Sumo (Remix) V</t>
+  </si>
+  <si>
+    <t>Sumo (Remix) VI</t>
+  </si>
+  <si>
+    <t>Sumo (Remix) VII</t>
+  </si>
+  <si>
+    <t>RPG vs Flying Cars</t>
+  </si>
+  <si>
+    <t>Stunters Vs Snipers - 4 Way</t>
+  </si>
+  <si>
+    <t>Duck Hunt OG</t>
+  </si>
+  <si>
+    <t>Hunting Pack I</t>
+  </si>
+  <si>
+    <t>Hunting Pack II</t>
+  </si>
+  <si>
+    <t>Hunting Pack III</t>
+  </si>
+  <si>
+    <t>Hunting Pack IV</t>
+  </si>
+  <si>
+    <t>Hunting Pack V</t>
+  </si>
+  <si>
+    <t>Hunting Pack VI</t>
+  </si>
+  <si>
+    <t>Hunting Pack VII</t>
   </si>
 </sst>
 </file>
@@ -450,15 +504,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6CBCF88-3E8A-41E4-B7E5-EBC293CC8BF6}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
@@ -467,122 +521,152 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D2">
         <v>8</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D3">
         <v>8</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>8</v>
+      </c>
+      <c r="E4">
         <v>3</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>36</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D5">
         <v>8</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>37</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D6">
         <v>8</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D7">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E7">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D8">
         <v>8</v>
       </c>
       <c r="E8">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="C9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E9">
         <v>2</v>
@@ -590,13 +674,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10">
         <v>8</v>
@@ -607,13 +691,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11">
         <v>8</v>
@@ -624,16 +708,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C12">
         <v>2</v>
       </c>
       <c r="D12">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E12">
         <v>2</v>
@@ -641,16 +725,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C13">
         <v>2</v>
       </c>
       <c r="D13">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E13">
         <v>2</v>
@@ -658,10 +742,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -675,16 +759,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C15">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D15">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E15">
         <v>2</v>
@@ -692,16 +776,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C16">
         <v>2</v>
       </c>
       <c r="D16">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="E16">
         <v>2</v>
@@ -709,19 +793,291 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>8</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>16</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>16</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20">
+        <v>8</v>
+      </c>
+      <c r="D20">
+        <v>16</v>
+      </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>18</v>
+      </c>
+      <c r="E21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>30</v>
+      </c>
+      <c r="E22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>18</v>
+      </c>
+      <c r="E23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <v>8</v>
+      </c>
+      <c r="E24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25">
+        <v>8</v>
+      </c>
+      <c r="E25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>21</v>
       </c>
-      <c r="B17" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17">
-        <v>2</v>
-      </c>
-      <c r="D17">
-        <v>18</v>
-      </c>
-      <c r="E17">
-        <v>2</v>
+      <c r="B26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26">
+        <v>8</v>
+      </c>
+      <c r="E26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27">
+        <v>16</v>
+      </c>
+      <c r="E27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28">
+        <v>16</v>
+      </c>
+      <c r="E28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <v>16</v>
+      </c>
+      <c r="E29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30">
+        <v>16</v>
+      </c>
+      <c r="E30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31">
+        <v>16</v>
+      </c>
+      <c r="E31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="D32">
+        <v>16</v>
+      </c>
+      <c r="E32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="D33">
+        <v>16</v>
+      </c>
+      <c r="E33">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>